<commit_message>
Expert Add Quiz Page Test Cases Added with Assertions
</commit_message>
<xml_diff>
--- a/AutomaticResumeFilter/src/resources/quizData.xlsx
+++ b/AutomaticResumeFilter/src/resources/quizData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthikck\IdeaProjects\Automatic-Resume-Filter-Automation\AutomaticResumeFilter\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C848B6-8384-4DE0-A4D8-2F32375FDAA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541896A4-3B07-4316-91A1-85B96DA7DF9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0E6AF072-9ED5-4BD7-9757-ED32F1E52CE1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
   <si>
     <t>Quiz Link</t>
   </si>
@@ -81,13 +81,25 @@
     <t>"01:00"</t>
   </si>
   <si>
-    <t>"0:00"</t>
-  </si>
-  <si>
     <t>"-01:00"</t>
   </si>
   <si>
     <t>"1.5"</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Recruitment Name</t>
+  </si>
+  <si>
+    <t>RECRUITMENT18</t>
+  </si>
+  <si>
+    <t>""</t>
   </si>
 </sst>
 </file>
@@ -467,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{594D6E86-4714-4B35-BEEC-51F14BDC3D99}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -478,9 +490,10 @@
     <col min="1" max="1" width="17.1796875" customWidth="1"/>
     <col min="2" max="2" width="13.08984375" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,8 +507,11 @@
         <v>3</v>
       </c>
       <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -508,8 +524,14 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -522,8 +544,11 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -536,8 +561,11 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -545,13 +573,16 @@
         <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -559,13 +590,16 @@
         <v>13</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -578,8 +612,11 @@
       <c r="D7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -587,13 +624,16 @@
         <v>12</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -606,8 +646,11 @@
       <c r="D9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -620,8 +663,11 @@
       <c r="D10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -634,9 +680,43 @@
       <c r="D11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C12" s="4"/>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -648,13 +728,21 @@
     <hyperlink ref="A11" r:id="rId6" xr:uid="{1994AABA-3C6C-4E17-B6BC-804B2E90D9F2}"/>
     <hyperlink ref="A6" r:id="rId7" xr:uid="{F3CAEDEE-06E0-45AF-9D3A-5E925263D23D}"/>
     <hyperlink ref="A5" r:id="rId8" xr:uid="{E4417B56-8E11-4453-9AB6-40DF851081C2}"/>
+    <hyperlink ref="A12" r:id="rId9" xr:uid="{0CAA2606-8389-4F6C-AE57-4CFF1938D79F}"/>
+    <hyperlink ref="A13" r:id="rId10" xr:uid="{B93B445B-CCE9-4AC3-8B78-3DEF90693AFF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005F941D346D0B5C49A26E58C2987129A3" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ba87752654f27b99cc8eef6b84ace69e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d309ed3e-2b68-4688-8e6b-753d07dea4f0" xmlns:ns4="1b3a36f9-9c01-4fe7-997e-4181a7cbcc1d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="035f1fc5589752c8fb69fe1342070459" ns3:_="" ns4:_="">
     <xsd:import namespace="d309ed3e-2b68-4688-8e6b-753d07dea4f0"/>
@@ -825,7 +913,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -834,13 +922,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3CDEB77-F605-48A6-9420-8F5FC52A0910}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1b3a36f9-9c01-4fe7-997e-4181a7cbcc1d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="d309ed3e-2b68-4688-8e6b-753d07dea4f0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98B27A80-C811-492F-A406-D71288010F76}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -859,27 +958,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF4E5EDD-E263-4E72-82B1-C84444367A90}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3CDEB77-F605-48A6-9420-8F5FC52A0910}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1b3a36f9-9c01-4fe7-997e-4181a7cbcc1d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="d309ed3e-2b68-4688-8e6b-753d07dea4f0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Expert Add Quiz Page Test Cases Updated
</commit_message>
<xml_diff>
--- a/AutomaticResumeFilter/src/resources/quizData.xlsx
+++ b/AutomaticResumeFilter/src/resources/quizData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthikck\IdeaProjects\Automatic-Resume-Filter-Automation\AutomaticResumeFilter\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541896A4-3B07-4316-91A1-85B96DA7DF9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BC9376-DD19-4168-BB48-282CFAA35111}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0E6AF072-9ED5-4BD7-9757-ED32F1E52CE1}"/>
   </bookViews>
@@ -96,10 +96,10 @@
     <t>Recruitment Name</t>
   </si>
   <si>
-    <t>RECRUITMENT18</t>
-  </si>
-  <si>
     <t>""</t>
+  </si>
+  <si>
+    <t>RECRUITMENT20</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -528,7 +528,7 @@
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -712,7 +712,7 @@
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Failure Test cases and logs added for Add quiz page
</commit_message>
<xml_diff>
--- a/AutomaticResumeFilter/src/resources/quizData.xlsx
+++ b/AutomaticResumeFilter/src/resources/quizData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashmittal2\Desktop\Automatic-Resume-Filter-Automation\AutomaticResumeFilter\src\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthikck\Desktop\Automation Testing\AutomaticResumeFilter\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40709D18-8785-4716-A8A5-1F1ECAA3A0DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5F994C-861C-4FFF-BFB9-AE9946C02A00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0E6AF072-9ED5-4BD7-9757-ED32F1E52CE1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="27">
   <si>
     <t>Quiz Link</t>
   </si>
@@ -60,33 +60,6 @@
     <t>"12345"</t>
   </si>
   <si>
-    <t>"5"</t>
-  </si>
-  <si>
-    <t>"0"</t>
-  </si>
-  <si>
-    <t>"5.5"</t>
-  </si>
-  <si>
-    <t>"-5"</t>
-  </si>
-  <si>
-    <t>"4/22/2022"</t>
-  </si>
-  <si>
-    <t>"3/15/2022"</t>
-  </si>
-  <si>
-    <t>"01:00"</t>
-  </si>
-  <si>
-    <t>"-01:00"</t>
-  </si>
-  <si>
-    <t>"1.5"</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -96,17 +69,59 @@
     <t>Recruitment Name</t>
   </si>
   <si>
-    <t>""</t>
-  </si>
-  <si>
-    <t>RECURIMENT2</t>
+    <t>4/22/2022</t>
+  </si>
+  <si>
+    <t>3/15/2022</t>
+  </si>
+  <si>
+    <t>01:00</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>-01:00</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>-5</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +141,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -152,18 +173,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -482,7 +504,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -508,217 +530,233 @@
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
+      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
-        <v>17</v>
+      <c r="F5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" t="s">
-        <v>17</v>
+      <c r="F6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="E7" t="s">
-        <v>17</v>
+      <c r="F7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
         <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="C9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
+      <c r="B10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
         <v>9</v>
-      </c>
-      <c r="E11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
         <v>8</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="B13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{60F080EF-C4C5-4DEF-856D-4D59EBBC6E15}"/>
     <hyperlink ref="A7" r:id="rId2" xr:uid="{379075F6-E902-4867-84BF-DEBDB48D7273}"/>
@@ -737,9 +775,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -914,27 +955,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3CDEB77-F605-48A6-9420-8F5FC52A0910}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF4E5EDD-E263-4E72-82B1-C84444367A90}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1b3a36f9-9c01-4fe7-997e-4181a7cbcc1d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="d309ed3e-2b68-4688-8e6b-753d07dea4f0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -959,9 +988,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF4E5EDD-E263-4E72-82B1-C84444367A90}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3CDEB77-F605-48A6-9420-8F5FC52A0910}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1b3a36f9-9c01-4fe7-997e-4181a7cbcc1d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="d309ed3e-2b68-4688-8e6b-753d07dea4f0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>